<commit_message>
Separate chem and pharma in BObIC, BEbIC, BVAbIC, and BECbIC
</commit_message>
<xml_diff>
--- a/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
+++ b/InputData/io-model/BECbIC/BAU Employee Compensation by ISIC Code.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\io-model\BECbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B79BD9-20AC-45FF-A8C3-5DA680E41FFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A8BAF-7035-4068-AE9D-CFE11F2ACEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4095" yWindow="870" windowWidth="24090" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="OECD VAL" sheetId="7" r:id="rId2"/>
-    <sheet name="BECbIC" sheetId="2" r:id="rId3"/>
+    <sheet name="OECD Chem Pharma Split" sheetId="8" r:id="rId3"/>
+    <sheet name="BECbIC" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -34,8 +35,616 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>MyOECD</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{EEF11BD2-AF37-4CBB-822E-6A31DF0D2344}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{DB22909D-6DEF-427A-9DE4-012C220EA4D1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{250E10D3-1062-4DD3-ACA2-ECD31EF86D7B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{BA4E2F55-F89E-4CFC-9D44-0D980255738F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{6A2248AB-FD7F-4D81-9017-AFD5A0BF36A5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{A657A8B0-625F-41D9-A714-633967FFC6AA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{59304A32-B30E-4E51-B733-34C77E61D8F4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{01AEFE9F-CB22-4E14-B29B-5B1045FB2935}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{69844961-6A1D-44CE-A62C-D4BDF93FD81B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L7" authorId="0" shapeId="0" xr:uid="{CC3DA8B0-C6A9-4FC0-9464-23612D864C1D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M7" authorId="0" shapeId="0" xr:uid="{6EBC89CE-CDF3-4665-9D22-CDE6F29F39C5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{CDFB8841-ECC7-4300-90CA-1CD3101EBBB0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{ABAA4756-53DB-4082-AFD1-0E5F7D4E45F4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{7361015B-B0DA-4571-B485-AE17B6D69348}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{4BC53B10-0905-45A1-AE44-F50D4A0C4A5B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{09020483-B8BF-4C53-A617-D6D6E77CA3E0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{C5FE7FCD-5AA6-4556-81BC-C1DD928FB394}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{17F6894A-A366-4E63-BD3A-DFD66672E41C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{C22E1DC1-1906-4A49-AF5B-36D228D6D95F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{C9F49FEE-1B73-4E82-8F43-D0AB5250B4F8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{0220E9A6-F15A-4287-9109-5CBB2B27001F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{084B4CAE-1EBC-46F1-B3BE-9203FAF4B7D0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{B0376147-BE58-4851-973A-B0A5603F664F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{10E6D036-E3E2-4F94-B0EA-043CBAFE02B0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{E0B12ECE-9AEB-40F4-82B8-48C064D764D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{84F3AC7D-9E1C-4EF2-8604-5316A64FDD6D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{DD5DD357-BE63-4807-951E-CCFF5A6E655F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{EAA92858-47E5-4D1B-B12B-FB56B8CD6ECD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{8FAC73F4-32CC-408C-8C48-42492CE55B0B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N19" authorId="0" shapeId="0" xr:uid="{745717A5-23A4-460A-AF67-28FC29A5900E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{FC3B65F3-BA75-4D9A-A934-1E78E0B182E5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{0FF52589-AF87-4D9C-895B-D0CF37A00CF9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{4DEEF721-454E-40EC-9786-9B45B2343B51}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{CB003191-E0E8-4796-8EBD-5444ABC3FB39}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{A15F6DA5-0F58-4DF2-A2A6-AC27212FE611}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{CDD17AE6-154C-4173-9DB9-1A37BC0BB3FC}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{97CC16F7-3884-4C49-B2A7-DC608CE55536}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="0" shapeId="0" xr:uid="{978EB612-BA98-4957-807A-042927E93D5E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{DA4E556F-AA80-4144-BE4A-F6F669C68038}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L20" authorId="0" shapeId="0" xr:uid="{D55C0177-370A-48F7-B7C1-CB557D77605D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">c: Estimates based on national Supply and Use tables (SUTs) or Input-Output tables </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M20" authorId="0" shapeId="0" xr:uid="{22D3F871-D7A1-4ACA-BC22-2720F77B2033}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N20" authorId="0" shapeId="0" xr:uid="{1C8FF4E3-5725-46AE-8C02-C328B0D8F32A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M29" authorId="0" shapeId="0" xr:uid="{BDC0603B-78F6-482E-ADEE-5D5119A63B9A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N29" authorId="0" shapeId="0" xr:uid="{00D23871-8CC2-4939-92F0-8A3E08254D64}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M31" authorId="0" shapeId="0" xr:uid="{A01148A4-EA42-4754-9899-49EECB140B83}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N31" authorId="0" shapeId="0" xr:uid="{414008A8-734C-4437-B821-6F20FAC93B94}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">b: Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4) </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="151">
   <si>
     <t>Source:</t>
   </si>
@@ -94,9 +703,6 @@
     <t>ISIC 19</t>
   </si>
   <si>
-    <t>ISIC 20T21</t>
-  </si>
-  <si>
     <t>ISIC 22</t>
   </si>
   <si>
@@ -175,9 +781,6 @@
     <t>ISIC 97T98</t>
   </si>
   <si>
-    <t>https://stats.oecd.org/Index.aspx?DataSetCode=IOTS#</t>
-  </si>
-  <si>
     <t>Dataset: Input-Output Tables 2018 edition</t>
   </si>
   <si>
@@ -341,6 +944,159 @@
   </si>
   <si>
     <t>BECbIC BAU Employee Compensation by ISIC Code</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;&lt;WebTableParameter xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://stats.oecd.org/OECDStatWS/2004/03/01/"&gt;&lt;DataTable Code="STANI4_2020" HasMetadata="true"&gt;&lt;Name LocaleIsoCode="en"&gt;STAN Industrial Analysis (2020 ed.)&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;STAN pour l'Analyse Structurelle (éd. 2020)&lt;/Name&gt;&lt;Dimension Code="LOCATION" HasMetadata="false" CommonCode="LOCATION" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Country&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pays&lt;/Name&gt;&lt;Member Code="AUS" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Australia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Australie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="AUT" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Austria&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Autriche&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="BEL" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Belgium&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Belgique&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CHL" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Chile&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Chili&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CZE" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Czech Republic&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;République tchèque&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="DNK" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Denmark&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Danemark&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="EST" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Estonia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Estonie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="FIN" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Finland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Finlande&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="FRA" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;France&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;France&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="DEU" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Germany&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Allemagne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="HUN" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Hungary&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Hongrie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ITA" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Italy&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Italie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="JPN" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Japan&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Japon&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="KOR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Korea&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Corée&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LVA" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Latvia&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Lettonie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LTU" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Lithuania&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Lituanie&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="MEX" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Mexico&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Mexique&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NLD" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Netherlands&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Pays-Bas&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="NOR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Norway&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Norvège&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="PRT" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Portugal&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Portugal&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="SVK" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Slovak Republic&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;République slovaque&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="ESP" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Spain&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Espagne&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="CHE" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Switzerland&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Suisse&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="GBR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;United Kingdom&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Royaume-Uni&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="USA" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;United States&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;États-Unis&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="VAR" HasMetadata="false" Display="codesandlabels"&gt;&lt;Name LocaleIsoCode="en"&gt;Variable&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Variable&lt;/Name&gt;&lt;Member Code="PROD" HasMetadata="true" HasOnlyUnitMetadata="true" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Production (gross output), current prices&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Production (brute), prix courants&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="VALU" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Value added, current prices&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Valeur ajoutée, prix courants&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="LABR" HasMetadata="true" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Labour costs (compensation of employees)&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Coût de la main-d'oeuvre (rémunération)&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="GOPS" HasMetadata="true" HasOnlyUnitMetadata="true" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Gross operating surplus and mixed income&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Excédent brut d'exploitation et revenu mixte&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="OTXS" HasMetadata="true" HasOnlyUnitMetadata="true" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Other taxes less subsidies on production&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Autres impôts moins subventions sur la production&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="EMPN" HasMetadata="true" HasOnlyUnitMetadata="true" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt;Number of persons engaged (total employment)&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Actifs occupés - emploi total&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="IND" HasMetadata="false" Display="codesandlabels"&gt;&lt;Name LocaleIsoCode="en"&gt;Industry&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Activité&lt;/Name&gt;&lt;Member Code="D20" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt; Chemicals and chemical products [CE]&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Produits chimiques [CE]&lt;/Name&gt;&lt;/Member&gt;&lt;Member Code="D21" HasMetadata="false" HasOnlyUnitMetadata="false" HasChild="0"&gt;&lt;Name LocaleIsoCode="en"&gt; Basic pharmaceutical products and pharmaceutical preparations [CF]&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Produits et préparations pharmaceutiques [CF]&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;Dimension Code="TIME" HasMetadata="false" CommonCode="TIME" Display="labels"&gt;&lt;Name LocaleIsoCode="en"&gt;Time&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;Temps&lt;/Name&gt;&lt;Member Code="2015" HasMetadata="false"&gt;&lt;Name LocaleIsoCode="en"&gt;2015&lt;/Name&gt;&lt;Name LocaleIsoCode="fr"&gt;2015&lt;/Name&gt;&lt;/Member&gt;&lt;/Dimension&gt;&lt;WBOSInformations&gt;&lt;TimeDimension WebTreeWasUsed="false"&gt;&lt;StartCodes Annual="2015" /&gt;&lt;EndCodes Annual="2015" /&gt;&lt;/TimeDimension&gt;&lt;/WBOSInformations&gt;&lt;Tabulation Axis="horizontal"&gt;&lt;Dimension Code="VAR" /&gt;&lt;Dimension Code="IND" /&gt;&lt;/Tabulation&gt;&lt;Tabulation Axis="vertical"&gt;&lt;Dimension Code="LOCATION" /&gt;&lt;/Tabulation&gt;&lt;Tabulation Axis="page"&gt;&lt;Dimension Code="TIME" /&gt;&lt;/Tabulation&gt;&lt;Formatting&gt;&lt;Labels LocaleIsoCode="en" /&gt;&lt;Power&gt;0&lt;/Power&gt;&lt;Decimals&gt;1&lt;/Decimals&gt;&lt;SkipEmptyLines&gt;true&lt;/SkipEmptyLines&gt;&lt;SkipEmptyCols&gt;false&lt;/SkipEmptyCols&gt;&lt;SkipLineHierarchy&gt;true&lt;/SkipLineHierarchy&gt;&lt;SkipColHierarchy&gt;false&lt;/SkipColHierarchy&gt;&lt;Page&gt;1&lt;/Page&gt;&lt;/Formatting&gt;&lt;/DataTable&gt;&lt;Format&gt;&lt;ShowEmptyAxes&gt;true&lt;/ShowEmptyAxes&gt;&lt;Page&gt;1&lt;/Page&gt;&lt;EnableSort&gt;true&lt;/EnableSort&gt;&lt;IncludeFlagColumn&gt;false&lt;/IncludeFlagColumn&gt;&lt;IncludeTimeSeriesId&gt;false&lt;/IncludeTimeSeriesId&gt;&lt;DoBarChart&gt;false&lt;/DoBarChart&gt;&lt;FreezePanes&gt;true&lt;/FreezePanes&gt;&lt;MaxBarChartLen&gt;65&lt;/MaxBarChartLen&gt;&lt;/Format&gt;&lt;Query&gt;&lt;AbsoluteUri&gt;http://stats.oecd.org//View.aspx?QueryId=&amp;amp;QueryType=Public&amp;amp;Lang=en&lt;/AbsoluteUri&gt;&lt;/Query&gt;&lt;/WebTableParameter&gt;</t>
+  </si>
+  <si>
+    <t>Dataset: STAN Industrial Analysis (2020 ed.)</t>
+  </si>
+  <si>
+    <t>PROD: Production (gross output), current prices</t>
+  </si>
+  <si>
+    <t>VALU: Value added, current prices</t>
+  </si>
+  <si>
+    <t>LABR: Labour costs (compensation of employees)</t>
+  </si>
+  <si>
+    <t>EMPN: Number of persons engaged (total employment)</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>D20: Chemicals and chemical products [CE]</t>
+  </si>
+  <si>
+    <t>D21: Basic pharmaceutical products and pharmaceutical preparations [CF]</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Slovak Republic</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Data extracted on 05 Oct 2020 23:14 UTC (GMT) from OECD.Stat</t>
+  </si>
+  <si>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t>c:</t>
+  </si>
+  <si>
+    <t>Estimates based on national Supply and Use tables (SUTs) or Input-Output tables</t>
+  </si>
+  <si>
+    <t>b:</t>
+  </si>
+  <si>
+    <t>Estimates based on detailed Structural Business Statistics (SBS) or industry census data: either published by OECD (ISIC Rev.4) and/or Eurostat (NACE Rev.2) or drawn directly from national sources (and converted from national industry classifications to ISIC Rev.4)</t>
+  </si>
+  <si>
+    <t>ISIC 20</t>
+  </si>
+  <si>
+    <t>ISIC 21</t>
+  </si>
+  <si>
+    <t>Most Industries</t>
+  </si>
+  <si>
+    <t>https://stats.oecd.org/Index.aspx?DataSetCode=IOTSI4_2018</t>
+  </si>
+  <si>
+    <t>Chemicals and Pharmaceuticals Industries</t>
+  </si>
+  <si>
+    <t>STAN Database for Structural Analysis</t>
+  </si>
+  <si>
+    <t>https://stats.oecd.org/Index.aspx?DataSetCode=STANI4_2020</t>
+  </si>
+  <si>
+    <t>Variable: PROD</t>
+  </si>
+  <si>
+    <t>We divide up chemicals and pharmaceuticals (ISIC 20T21) into separate chemicals (ISIC 20)</t>
+  </si>
+  <si>
+    <t>and pharmaceuticals (ISIC 21) industries using data from a different OECD database.</t>
   </si>
 </sst>
 </file>
@@ -351,7 +1107,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,8 +1201,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +1242,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F8FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,7 +1324,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -620,6 +1394,72 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -902,7 +1742,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -913,71 +1753,117 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="50" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="50" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>0.9686815713640794</v>
+      </c>
+      <c r="B25" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>0.9686815713640794</v>
-      </c>
-      <c r="B14" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="https://stats.oecd.org/Index.aspx?DataSetCode=IOTS" xr:uid="{C45F7FD1-E582-4900-94D0-FDF23F149E19}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{676EE023-F1C0-4717-8897-C81C92D54826}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{738871AA-8A85-449E-9916-DE46D7228F91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1014,16 +1900,16 @@
     </row>
     <row r="2" spans="1:38" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
@@ -1155,7 +2041,7 @@
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -1195,121 +2081,121 @@
     </row>
     <row r="7" spans="1:38" ht="126" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="F7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="G7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="J7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="L7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="N7" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="P7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="Q7" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="R7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="S7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="T7" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="U7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="T7" s="8" t="s">
+      <c r="V7" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="W7" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="V7" s="8" t="s">
+      <c r="X7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="W7" s="8" t="s">
+      <c r="Y7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="X7" s="8" t="s">
+      <c r="Z7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="AA7" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="AB7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AC7" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AE7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AF7" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AH7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AI7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AH7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AK7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="AJ7" s="8" t="s">
+      <c r="AL7" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="AK7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL7" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>9</v>
@@ -1425,7 +2311,7 @@
     </row>
     <row r="9" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
@@ -1541,7 +2427,7 @@
     </row>
     <row r="10" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>9</v>
@@ -1657,7 +2543,7 @@
     </row>
     <row r="11" spans="1:38" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>9</v>
@@ -1773,7 +2659,7 @@
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1799,23 +2685,1366 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E446F6-C76E-49FD-A090-AD4B65FAC91F}">
+  <dimension ref="A1:N35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" customWidth="1"/>
+    <col min="3" max="14" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="e">
+        <f ca="1">DotStatQuery(B1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+    </row>
+    <row r="4" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="37"/>
+      <c r="G4" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="37"/>
+      <c r="I4" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="37"/>
+      <c r="M4" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" s="37"/>
+    </row>
+    <row r="5" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="42">
+        <v>17390</v>
+      </c>
+      <c r="D7" s="42">
+        <v>10427</v>
+      </c>
+      <c r="E7" s="42">
+        <v>6061</v>
+      </c>
+      <c r="F7" s="42">
+        <v>3451</v>
+      </c>
+      <c r="G7" s="42">
+        <v>2949</v>
+      </c>
+      <c r="H7" s="42">
+        <v>1466</v>
+      </c>
+      <c r="I7" s="42">
+        <v>2957</v>
+      </c>
+      <c r="J7" s="42">
+        <v>1941</v>
+      </c>
+      <c r="K7" s="42">
+        <v>151</v>
+      </c>
+      <c r="L7" s="42">
+        <v>48</v>
+      </c>
+      <c r="M7" s="42">
+        <v>31.715</v>
+      </c>
+      <c r="N7" s="42">
+        <v>16.427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="43">
+        <v>13142.207</v>
+      </c>
+      <c r="D8" s="43">
+        <v>4268.8580000000002</v>
+      </c>
+      <c r="E8" s="43">
+        <v>2750.683</v>
+      </c>
+      <c r="F8" s="43">
+        <v>2190.2440000000001</v>
+      </c>
+      <c r="G8" s="43">
+        <v>1169.6790000000001</v>
+      </c>
+      <c r="H8" s="43">
+        <v>999.32500000000005</v>
+      </c>
+      <c r="I8" s="43">
+        <v>1540.5920000000001</v>
+      </c>
+      <c r="J8" s="43">
+        <v>1143.9290000000001</v>
+      </c>
+      <c r="K8" s="43">
+        <v>40.411999999999999</v>
+      </c>
+      <c r="L8" s="43">
+        <v>46.99</v>
+      </c>
+      <c r="M8" s="43">
+        <v>17.47</v>
+      </c>
+      <c r="N8" s="43">
+        <v>15.18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="42">
+        <v>32184.7</v>
+      </c>
+      <c r="D9" s="42">
+        <v>15967.8</v>
+      </c>
+      <c r="E9" s="42">
+        <v>9208.1</v>
+      </c>
+      <c r="F9" s="42">
+        <v>5799.6</v>
+      </c>
+      <c r="G9" s="42">
+        <v>4169.7</v>
+      </c>
+      <c r="H9" s="42">
+        <v>2219.6999999999998</v>
+      </c>
+      <c r="I9" s="42">
+        <v>5127.8</v>
+      </c>
+      <c r="J9" s="42">
+        <v>3664</v>
+      </c>
+      <c r="K9" s="42">
+        <v>-89.4</v>
+      </c>
+      <c r="L9" s="42">
+        <v>-84.1</v>
+      </c>
+      <c r="M9" s="42">
+        <v>44</v>
+      </c>
+      <c r="N9" s="42">
+        <v>23.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="43">
+        <v>4296151.79</v>
+      </c>
+      <c r="D10" s="43">
+        <v>1176806.6969999999</v>
+      </c>
+      <c r="E10" s="43">
+        <v>1262313.6129999999</v>
+      </c>
+      <c r="F10" s="43">
+        <v>414529.82299999997</v>
+      </c>
+      <c r="G10" s="43">
+        <v>410617.86</v>
+      </c>
+      <c r="H10" s="43">
+        <v>197186.617</v>
+      </c>
+      <c r="I10" s="43">
+        <v>825702.42099999997</v>
+      </c>
+      <c r="J10" s="43">
+        <v>207059.06099999999</v>
+      </c>
+      <c r="K10" s="43">
+        <v>25993.348999999998</v>
+      </c>
+      <c r="L10" s="43">
+        <v>10284.14</v>
+      </c>
+      <c r="M10" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="N10" s="43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="42">
+        <v>155577</v>
+      </c>
+      <c r="D11" s="42">
+        <v>41847</v>
+      </c>
+      <c r="E11" s="42">
+        <v>40096</v>
+      </c>
+      <c r="F11" s="42">
+        <v>17707</v>
+      </c>
+      <c r="G11" s="42">
+        <v>14359</v>
+      </c>
+      <c r="H11" s="42">
+        <v>4980</v>
+      </c>
+      <c r="I11" s="42">
+        <v>25779</v>
+      </c>
+      <c r="J11" s="42">
+        <v>12717</v>
+      </c>
+      <c r="K11" s="42">
+        <v>-42</v>
+      </c>
+      <c r="L11" s="42">
+        <v>10</v>
+      </c>
+      <c r="M11" s="42">
+        <v>30.922000000000001</v>
+      </c>
+      <c r="N11" s="42">
+        <v>11.698</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="43">
+        <v>41360</v>
+      </c>
+      <c r="D12" s="43">
+        <v>92114</v>
+      </c>
+      <c r="E12" s="43">
+        <v>18022</v>
+      </c>
+      <c r="F12" s="43">
+        <v>60233</v>
+      </c>
+      <c r="G12" s="43">
+        <v>6417</v>
+      </c>
+      <c r="H12" s="43">
+        <v>16429</v>
+      </c>
+      <c r="I12" s="43">
+        <v>11520</v>
+      </c>
+      <c r="J12" s="43">
+        <v>43707</v>
+      </c>
+      <c r="K12" s="43">
+        <v>85</v>
+      </c>
+      <c r="L12" s="43">
+        <v>98</v>
+      </c>
+      <c r="M12" s="43">
+        <v>11.451000000000001</v>
+      </c>
+      <c r="N12" s="43">
+        <v>22.722000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="42">
+        <v>429.8</v>
+      </c>
+      <c r="D13" s="42">
+        <v>45.4</v>
+      </c>
+      <c r="E13" s="42">
+        <v>106.1</v>
+      </c>
+      <c r="F13" s="42">
+        <v>11</v>
+      </c>
+      <c r="G13" s="42">
+        <v>50.2</v>
+      </c>
+      <c r="H13" s="42">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I13" s="42">
+        <v>56</v>
+      </c>
+      <c r="J13" s="42">
+        <v>1.8</v>
+      </c>
+      <c r="K13" s="42">
+        <v>-0.1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>0</v>
+      </c>
+      <c r="M13" s="42">
+        <v>3.1</v>
+      </c>
+      <c r="N13" s="42">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="43">
+        <v>7559</v>
+      </c>
+      <c r="D14" s="43">
+        <v>1835</v>
+      </c>
+      <c r="E14" s="43">
+        <v>2022</v>
+      </c>
+      <c r="F14" s="43">
+        <v>1315</v>
+      </c>
+      <c r="G14" s="43">
+        <v>775</v>
+      </c>
+      <c r="H14" s="43">
+        <v>264</v>
+      </c>
+      <c r="I14" s="43">
+        <v>1266</v>
+      </c>
+      <c r="J14" s="43">
+        <v>1056</v>
+      </c>
+      <c r="K14" s="43">
+        <v>-19</v>
+      </c>
+      <c r="L14" s="43">
+        <v>-5</v>
+      </c>
+      <c r="M14" s="43">
+        <v>12.8</v>
+      </c>
+      <c r="N14" s="43">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="42">
+        <v>64869</v>
+      </c>
+      <c r="D15" s="42">
+        <v>26029</v>
+      </c>
+      <c r="E15" s="42">
+        <v>19595</v>
+      </c>
+      <c r="F15" s="42">
+        <v>12412</v>
+      </c>
+      <c r="G15" s="42">
+        <v>8882</v>
+      </c>
+      <c r="H15" s="42">
+        <v>4218</v>
+      </c>
+      <c r="I15" s="42">
+        <v>9941</v>
+      </c>
+      <c r="J15" s="42">
+        <v>7853</v>
+      </c>
+      <c r="K15" s="42">
+        <v>772</v>
+      </c>
+      <c r="L15" s="42">
+        <v>341</v>
+      </c>
+      <c r="M15" s="42">
+        <v>111</v>
+      </c>
+      <c r="N15" s="42">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="43">
+        <v>137727</v>
+      </c>
+      <c r="D16" s="43">
+        <v>46535</v>
+      </c>
+      <c r="E16" s="43">
+        <v>45580</v>
+      </c>
+      <c r="F16" s="43">
+        <v>22858</v>
+      </c>
+      <c r="G16" s="43">
+        <v>24028</v>
+      </c>
+      <c r="H16" s="43">
+        <v>8909</v>
+      </c>
+      <c r="I16" s="43">
+        <v>21374</v>
+      </c>
+      <c r="J16" s="43">
+        <v>13883</v>
+      </c>
+      <c r="K16" s="43">
+        <v>178</v>
+      </c>
+      <c r="L16" s="43">
+        <v>66</v>
+      </c>
+      <c r="M16" s="43">
+        <v>348</v>
+      </c>
+      <c r="N16" s="43">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="42">
+        <v>1561214</v>
+      </c>
+      <c r="D17" s="42">
+        <v>950652</v>
+      </c>
+      <c r="E17" s="42">
+        <v>392029</v>
+      </c>
+      <c r="F17" s="42">
+        <v>450794</v>
+      </c>
+      <c r="G17" s="42">
+        <v>89594</v>
+      </c>
+      <c r="H17" s="42">
+        <v>149504</v>
+      </c>
+      <c r="I17" s="42">
+        <v>294084</v>
+      </c>
+      <c r="J17" s="42">
+        <v>298569</v>
+      </c>
+      <c r="K17" s="42">
+        <v>8351</v>
+      </c>
+      <c r="L17" s="42">
+        <v>2721</v>
+      </c>
+      <c r="M17" s="42">
+        <v>16.291</v>
+      </c>
+      <c r="N17" s="42">
+        <v>20.789000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="43">
+        <v>50506.5</v>
+      </c>
+      <c r="D18" s="43">
+        <v>25044.1</v>
+      </c>
+      <c r="E18" s="43">
+        <v>10896.2</v>
+      </c>
+      <c r="F18" s="43">
+        <v>8888.5</v>
+      </c>
+      <c r="G18" s="43">
+        <v>5723.3</v>
+      </c>
+      <c r="H18" s="43">
+        <v>4034.3</v>
+      </c>
+      <c r="I18" s="43">
+        <v>4864.1000000000004</v>
+      </c>
+      <c r="J18" s="43">
+        <v>4486.5</v>
+      </c>
+      <c r="K18" s="43">
+        <v>308.8</v>
+      </c>
+      <c r="L18" s="43">
+        <v>367.7</v>
+      </c>
+      <c r="M18" s="43">
+        <v>109.7</v>
+      </c>
+      <c r="N18" s="43">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="42">
+        <v>22424500</v>
+      </c>
+      <c r="D19" s="42">
+        <v>9255400</v>
+      </c>
+      <c r="E19" s="42">
+        <v>8516400</v>
+      </c>
+      <c r="F19" s="42">
+        <v>3015900</v>
+      </c>
+      <c r="G19" s="42">
+        <v>2266700</v>
+      </c>
+      <c r="H19" s="42">
+        <v>802700</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="K19" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="M19" s="42">
+        <v>328</v>
+      </c>
+      <c r="N19" s="42">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="43">
+        <v>144820316</v>
+      </c>
+      <c r="D20" s="43">
+        <v>17629352</v>
+      </c>
+      <c r="E20" s="43">
+        <v>38090317</v>
+      </c>
+      <c r="F20" s="43">
+        <v>6699394</v>
+      </c>
+      <c r="G20" s="43">
+        <v>9391789</v>
+      </c>
+      <c r="H20" s="43">
+        <v>1980796</v>
+      </c>
+      <c r="I20" s="43">
+        <v>28334763</v>
+      </c>
+      <c r="J20" s="43">
+        <v>4673860</v>
+      </c>
+      <c r="K20" s="43">
+        <v>363765</v>
+      </c>
+      <c r="L20" s="43">
+        <v>44738</v>
+      </c>
+      <c r="M20" s="43">
+        <v>175.2</v>
+      </c>
+      <c r="N20" s="43">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="42">
+        <v>245.93</v>
+      </c>
+      <c r="D21" s="42">
+        <v>156.44999999999999</v>
+      </c>
+      <c r="E21" s="42">
+        <v>61.082999999999998</v>
+      </c>
+      <c r="F21" s="42">
+        <v>78.703999999999994</v>
+      </c>
+      <c r="G21" s="42">
+        <v>33.743000000000002</v>
+      </c>
+      <c r="H21" s="42">
+        <v>41.521000000000001</v>
+      </c>
+      <c r="I21" s="42">
+        <v>26.463999999999999</v>
+      </c>
+      <c r="J21" s="42">
+        <v>36.499000000000002</v>
+      </c>
+      <c r="K21" s="42">
+        <v>0.876</v>
+      </c>
+      <c r="L21" s="42">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="M21" s="42">
+        <v>2.8730000000000002</v>
+      </c>
+      <c r="N21" s="42">
+        <v>2.351</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="43">
+        <v>2026.5</v>
+      </c>
+      <c r="D22" s="43">
+        <v>215.7</v>
+      </c>
+      <c r="E22" s="43">
+        <v>532.5</v>
+      </c>
+      <c r="F22" s="43">
+        <v>169.2</v>
+      </c>
+      <c r="G22" s="43">
+        <v>126.7</v>
+      </c>
+      <c r="H22" s="43">
+        <v>17.5</v>
+      </c>
+      <c r="I22" s="43">
+        <v>407.4</v>
+      </c>
+      <c r="J22" s="43">
+        <v>151.69999999999999</v>
+      </c>
+      <c r="K22" s="43">
+        <v>-1.5</v>
+      </c>
+      <c r="L22" s="43">
+        <v>0.1</v>
+      </c>
+      <c r="M22" s="43">
+        <v>6.6</v>
+      </c>
+      <c r="N22" s="43">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="42">
+        <v>720647.26100000006</v>
+      </c>
+      <c r="D23" s="42">
+        <v>275739.48700000002</v>
+      </c>
+      <c r="E23" s="42">
+        <v>210925.78400000001</v>
+      </c>
+      <c r="F23" s="42">
+        <v>65884.478000000003</v>
+      </c>
+      <c r="G23" s="42">
+        <v>38561.97</v>
+      </c>
+      <c r="H23" s="42">
+        <v>25493.957999999999</v>
+      </c>
+      <c r="I23" s="42">
+        <v>170135.56</v>
+      </c>
+      <c r="J23" s="42">
+        <v>39511.928999999996</v>
+      </c>
+      <c r="K23" s="42">
+        <v>2228.2539999999999</v>
+      </c>
+      <c r="L23" s="42">
+        <v>878.59100000000001</v>
+      </c>
+      <c r="M23" s="42">
+        <v>155.35499999999999</v>
+      </c>
+      <c r="N23" s="42">
+        <v>118.422</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="43">
+        <v>41782</v>
+      </c>
+      <c r="D24" s="43">
+        <v>5784</v>
+      </c>
+      <c r="E24" s="43">
+        <v>9497</v>
+      </c>
+      <c r="F24" s="43">
+        <v>2423</v>
+      </c>
+      <c r="G24" s="43">
+        <v>3475</v>
+      </c>
+      <c r="H24" s="43">
+        <v>902</v>
+      </c>
+      <c r="I24" s="43">
+        <v>6007</v>
+      </c>
+      <c r="J24" s="43">
+        <v>1552</v>
+      </c>
+      <c r="K24" s="43">
+        <v>15</v>
+      </c>
+      <c r="L24" s="43">
+        <v>-31</v>
+      </c>
+      <c r="M24" s="43">
+        <v>43</v>
+      </c>
+      <c r="N24" s="43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="42">
+        <v>56741</v>
+      </c>
+      <c r="D25" s="42">
+        <v>12448</v>
+      </c>
+      <c r="E25" s="42">
+        <v>15300</v>
+      </c>
+      <c r="F25" s="42">
+        <v>6492</v>
+      </c>
+      <c r="G25" s="42">
+        <v>7609</v>
+      </c>
+      <c r="H25" s="42">
+        <v>2019</v>
+      </c>
+      <c r="I25" s="42">
+        <v>7709</v>
+      </c>
+      <c r="J25" s="42">
+        <v>4473</v>
+      </c>
+      <c r="K25" s="42">
+        <v>-18</v>
+      </c>
+      <c r="L25" s="42">
+        <v>0</v>
+      </c>
+      <c r="M25" s="42">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="N25" s="42">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="43">
+        <v>4356.4840000000004</v>
+      </c>
+      <c r="D26" s="43">
+        <v>1175.9290000000001</v>
+      </c>
+      <c r="E26" s="43">
+        <v>878.67700000000002</v>
+      </c>
+      <c r="F26" s="43">
+        <v>505.16399999999999</v>
+      </c>
+      <c r="G26" s="43">
+        <v>356.76100000000002</v>
+      </c>
+      <c r="H26" s="43">
+        <v>204.215</v>
+      </c>
+      <c r="I26" s="43">
+        <v>503.59199999999998</v>
+      </c>
+      <c r="J26" s="43">
+        <v>225.114</v>
+      </c>
+      <c r="K26" s="43">
+        <v>18.324000000000002</v>
+      </c>
+      <c r="L26" s="43">
+        <v>75.834999999999994</v>
+      </c>
+      <c r="M26" s="43">
+        <v>12.057</v>
+      </c>
+      <c r="N26" s="43">
+        <v>6.2270000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="42">
+        <v>1907.855</v>
+      </c>
+      <c r="D27" s="42">
+        <v>209.029</v>
+      </c>
+      <c r="E27" s="42">
+        <v>646.14</v>
+      </c>
+      <c r="F27" s="42">
+        <v>55.09</v>
+      </c>
+      <c r="G27" s="42">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="H27" s="42">
+        <v>45.83</v>
+      </c>
+      <c r="I27" s="42">
+        <v>492.09699999999998</v>
+      </c>
+      <c r="J27" s="42">
+        <v>9.3350000000000009</v>
+      </c>
+      <c r="K27" s="42">
+        <v>-2.2650000000000001</v>
+      </c>
+      <c r="L27" s="42">
+        <v>-7.2999999999999995E-2</v>
+      </c>
+      <c r="M27" s="42">
+        <v>8.5920000000000005</v>
+      </c>
+      <c r="N27" s="42">
+        <v>2.2280000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="43">
+        <v>36741</v>
+      </c>
+      <c r="D28" s="43">
+        <v>15161</v>
+      </c>
+      <c r="E28" s="43">
+        <v>8061</v>
+      </c>
+      <c r="F28" s="43">
+        <v>6833</v>
+      </c>
+      <c r="G28" s="43">
+        <v>3954</v>
+      </c>
+      <c r="H28" s="43">
+        <v>2115</v>
+      </c>
+      <c r="I28" s="43">
+        <v>4057</v>
+      </c>
+      <c r="J28" s="43">
+        <v>4711</v>
+      </c>
+      <c r="K28" s="43">
+        <v>50</v>
+      </c>
+      <c r="L28" s="43">
+        <v>7</v>
+      </c>
+      <c r="M28" s="43">
+        <v>83.8</v>
+      </c>
+      <c r="N28" s="43">
+        <v>39.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="42">
+        <v>23031.416700000002</v>
+      </c>
+      <c r="D29" s="42">
+        <v>80032.204400000002</v>
+      </c>
+      <c r="E29" s="42">
+        <v>7470.1342000000004</v>
+      </c>
+      <c r="F29" s="42">
+        <v>28686.775900000001</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="H29" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="I29" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="J29" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="L29" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="M29" s="42">
+        <v>29.100999999999999</v>
+      </c>
+      <c r="N29" s="42">
+        <v>46.713000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="43">
+        <v>32794</v>
+      </c>
+      <c r="D30" s="43">
+        <v>21282</v>
+      </c>
+      <c r="E30" s="43">
+        <v>12217</v>
+      </c>
+      <c r="F30" s="43">
+        <v>11848</v>
+      </c>
+      <c r="G30" s="43">
+        <v>6748</v>
+      </c>
+      <c r="H30" s="43">
+        <v>4114</v>
+      </c>
+      <c r="I30" s="43">
+        <v>5410</v>
+      </c>
+      <c r="J30" s="43">
+        <v>7721</v>
+      </c>
+      <c r="K30" s="43">
+        <v>59</v>
+      </c>
+      <c r="L30" s="43">
+        <v>13</v>
+      </c>
+      <c r="M30" s="43">
+        <v>96.19</v>
+      </c>
+      <c r="N30" s="43">
+        <v>40.64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="42">
+        <v>515221</v>
+      </c>
+      <c r="D31" s="42">
+        <v>266206</v>
+      </c>
+      <c r="E31" s="42">
+        <v>184192</v>
+      </c>
+      <c r="F31" s="42">
+        <v>143569</v>
+      </c>
+      <c r="G31" s="42">
+        <v>54606</v>
+      </c>
+      <c r="H31" s="42">
+        <v>45877</v>
+      </c>
+      <c r="I31" s="42">
+        <v>120465</v>
+      </c>
+      <c r="J31" s="42">
+        <v>94460</v>
+      </c>
+      <c r="K31" s="42">
+        <v>9121</v>
+      </c>
+      <c r="L31" s="42">
+        <v>3232</v>
+      </c>
+      <c r="M31" s="42">
+        <v>534</v>
+      </c>
+      <c r="N31" s="42">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{74C1BA66-5936-4644-B930-C4F144CD2C37}"/>
+    <hyperlink ref="C4" r:id="rId2" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[VAR].[PROD]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{8DE88401-0FB2-4F1C-A552-8C5ECA6A140E}"/>
+    <hyperlink ref="E4" r:id="rId3" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[VAR].[VALU]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{82BCB2A3-769A-486B-887F-FED847CB24F0}"/>
+    <hyperlink ref="G4" r:id="rId4" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[VAR].[LABR]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{BD1EA945-C1A9-41BE-B3D2-C9DB44FD5713}"/>
+    <hyperlink ref="I4" r:id="rId5" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[VAR].[GOPS]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{767D0A57-EC49-41F9-A009-9A37D95370EA}"/>
+    <hyperlink ref="K4" r:id="rId6" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[VAR].[OTXS]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{F535E580-F99E-460C-9B95-C624903E7FC0}"/>
+    <hyperlink ref="M4" r:id="rId7" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[VAR].[EMPN]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{307224DE-A381-4D9A-9E5C-149AF929770D}"/>
+    <hyperlink ref="A7" r:id="rId8" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[AUS]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{EE6B1FA3-84F1-4D4E-B386-FD2C2851185E}"/>
+    <hyperlink ref="A8" r:id="rId9" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[AUT]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{70860490-4592-4EC0-89ED-68E139694E30}"/>
+    <hyperlink ref="A9" r:id="rId10" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[BEL]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{E2AE1E65-84D0-4C4D-AA14-199A14480412}"/>
+    <hyperlink ref="A10" r:id="rId11" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[CHL]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{65F82E61-E422-4437-9AB9-A36824FB8672}"/>
+    <hyperlink ref="A11" r:id="rId12" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[CZE]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{C5C32C9B-67CD-4896-8214-0C7C6E039CBE}"/>
+    <hyperlink ref="A12" r:id="rId13" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[DNK]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{FA7D9339-A2C1-42D9-8295-C08CF00EBA32}"/>
+    <hyperlink ref="A13" r:id="rId14" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[EST]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{7E892E7C-7BCE-4BB7-828F-C7D0C1D170A6}"/>
+    <hyperlink ref="A14" r:id="rId15" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[FIN]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{7B947448-4315-4692-B9E0-5235A88947F3}"/>
+    <hyperlink ref="A15" r:id="rId16" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[FRA]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{9F4052D8-FC15-488C-8392-4788E082A26D}"/>
+    <hyperlink ref="A16" r:id="rId17" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[DEU]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{5A0641A9-8316-4480-BE2D-C0A44D851655}"/>
+    <hyperlink ref="A17" r:id="rId18" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[HUN]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{165828BF-7CCB-4860-B20C-A8A1D460691E}"/>
+    <hyperlink ref="A18" r:id="rId19" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[ITA]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{2D2C4FF1-931B-4340-8CF8-9E356B5A417C}"/>
+    <hyperlink ref="A19" r:id="rId20" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[JPN]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{F8D2D72B-9AA0-4F5A-8818-21F461B79B2D}"/>
+    <hyperlink ref="A20" r:id="rId21" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[KOR]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{F2752334-8175-4E6B-9218-427B79DF3C2C}"/>
+    <hyperlink ref="A21" r:id="rId22" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[LVA]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{E1ED38D3-4633-4B3E-B62F-8D9C5B310ACC}"/>
+    <hyperlink ref="A23" r:id="rId23" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[MEX]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{30D159F1-1D49-4393-B207-F663CAD54CF5}"/>
+    <hyperlink ref="A24" r:id="rId24" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[NLD]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{DF088931-826D-435C-B084-93A9D6C77123}"/>
+    <hyperlink ref="A25" r:id="rId25" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[NOR]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{91D8E8A9-9A1C-4B13-97CB-3C7139A8FD74}"/>
+    <hyperlink ref="A26" r:id="rId26" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[PRT]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{DC31E0C0-0794-4B4E-9883-33FE19CBFA5F}"/>
+    <hyperlink ref="A27" r:id="rId27" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=%5bLOCATION%5d.%5bSVK%5d&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{D961BCF6-9328-4431-84A6-8CD85AEBD014}"/>
+    <hyperlink ref="A28" r:id="rId28" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[ESP]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{60AAD49C-7E2A-437E-BB04-C5783C129049}"/>
+    <hyperlink ref="A29" r:id="rId29" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[CHE]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{DCF3B3D2-3691-4CF0-B62C-F98616572417}"/>
+    <hyperlink ref="A30" r:id="rId30" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[GBR]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{8027E701-4B8E-4B32-9621-BE5C05E55FDD}"/>
+    <hyperlink ref="A31" r:id="rId31" display="http://stats.oecd.org/OECDStat_Metadata/ShowMetadata.ashx?Dataset=STANI4_2020&amp;Coords=[LOCATION].[USA]&amp;ShowOnWeb=true&amp;Lang=en" xr:uid="{23B11085-6D89-4C27-9ABE-24B45E60ECC9}"/>
+    <hyperlink ref="A32" r:id="rId32" display="https://stats-2.oecd.org/index.aspx?DatasetCode=STANI4_2020" xr:uid="{626315FD-378A-45C5-BAFF-D9FE99FF0746}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId33"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="37" width="10.140625" customWidth="1"/>
+    <col min="2" max="38" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -1844,234 +4073,241 @@
       <c r="J1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2">
-        <f>'OECD VAL'!C9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!C9*10^6*About!$A$25</f>
         <v>54016507157.360023</v>
       </c>
       <c r="C2">
-        <f>'OECD VAL'!D9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!D9*10^6*About!$A$25</f>
         <v>42087940459.502907</v>
       </c>
       <c r="D2">
-        <f>'OECD VAL'!E9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!E9*10^6*About!$A$25</f>
         <v>13192667088.040098</v>
       </c>
       <c r="E2">
-        <f>'OECD VAL'!F9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!F9*10^6*About!$A$25</f>
         <v>31699803162.920803</v>
       </c>
       <c r="F2">
-        <f>'OECD VAL'!G9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!G9*10^6*About!$A$25</f>
         <v>104565156568.91278</v>
       </c>
       <c r="G2">
-        <f>'OECD VAL'!H9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!H9*10^6*About!$A$25</f>
         <v>19249581096.571133</v>
       </c>
       <c r="H2">
-        <f>'OECD VAL'!I9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!I9*10^6*About!$A$25</f>
         <v>19084921697.025951</v>
       </c>
       <c r="I2">
-        <f>'OECD VAL'!J9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!J9*10^6*About!$A$25</f>
         <v>53950867356.721252</v>
       </c>
       <c r="J2">
-        <f>'OECD VAL'!K9*10^6*About!$A$14</f>
+        <f>'OECD VAL'!K9*10^6*About!$A$25</f>
         <v>17895825352.232121</v>
       </c>
-      <c r="K2">
-        <f>'OECD VAL'!L9*10^6*About!$A$14</f>
-        <v>97892958305.927429</v>
-      </c>
-      <c r="L2">
-        <f>'OECD VAL'!M9*10^6*About!$A$14</f>
+      <c r="K2" s="49">
+        <f>'OECD VAL'!L9*10^6*About!$A$25*('OECD Chem Pharma Split'!G$31/SUM('OECD Chem Pharma Split'!$G$31:$H$31))</f>
+        <v>53198480153.393837</v>
+      </c>
+      <c r="L2" s="49">
+        <f>'OECD VAL'!L9*10^6*About!$A$25*('OECD Chem Pharma Split'!H$31/SUM('OECD Chem Pharma Split'!$G$31:$H$31))</f>
+        <v>44694478152.533585</v>
+      </c>
+      <c r="M2">
+        <f>'OECD VAL'!M9*10^6*About!$A$25</f>
         <v>48035143530.62439</v>
       </c>
-      <c r="M2">
-        <f>'OECD VAL'!N9*10^6*About!$A$14</f>
+      <c r="N2">
+        <f>'OECD VAL'!N9*10^6*About!$A$25</f>
         <v>27963696179.008259</v>
       </c>
-      <c r="N2">
-        <f>'OECD VAL'!O9*10^6*About!$A$14</f>
+      <c r="O2">
+        <f>'OECD VAL'!O9*10^6*About!$A$25</f>
         <v>30535090470.641346</v>
       </c>
-      <c r="O2">
-        <f>'OECD VAL'!P9*10^6*About!$A$14</f>
+      <c r="P2">
+        <f>'OECD VAL'!P9*10^6*About!$A$25</f>
         <v>93149679188.412643</v>
       </c>
-      <c r="P2">
-        <f>'OECD VAL'!Q9*10^6*About!$A$14</f>
+      <c r="Q2">
+        <f>'OECD VAL'!Q9*10^6*About!$A$25</f>
         <v>133807960921.68916</v>
       </c>
-      <c r="Q2">
-        <f>'OECD VAL'!R9*10^6*About!$A$14</f>
+      <c r="R2">
+        <f>'OECD VAL'!R9*10^6*About!$A$25</f>
         <v>33053576343.528103</v>
       </c>
-      <c r="R2">
-        <f>'OECD VAL'!S9*10^6*About!$A$14</f>
+      <c r="S2">
+        <f>'OECD VAL'!S9*10^6*About!$A$25</f>
         <v>87657629558.546432</v>
       </c>
-      <c r="S2">
-        <f>'OECD VAL'!T9*10^6*About!$A$14</f>
+      <c r="T2">
+        <f>'OECD VAL'!T9*10^6*About!$A$25</f>
         <v>66099176562.997589</v>
       </c>
-      <c r="T2">
-        <f>'OECD VAL'!U9*10^6*About!$A$14</f>
+      <c r="U2">
+        <f>'OECD VAL'!U9*10^6*About!$A$25</f>
         <v>76755469135.572556</v>
       </c>
-      <c r="U2">
-        <f>'OECD VAL'!V9*10^6*About!$A$14</f>
+      <c r="V2">
+        <f>'OECD VAL'!V9*10^6*About!$A$25</f>
         <v>70758876865.8535</v>
       </c>
-      <c r="V2">
-        <f>'OECD VAL'!W9*10^6*About!$A$14</f>
+      <c r="W2">
+        <f>'OECD VAL'!W9*10^6*About!$A$25</f>
         <v>99649765984.524323</v>
       </c>
-      <c r="W2">
-        <f>'OECD VAL'!X9*10^6*About!$A$14</f>
+      <c r="X2">
+        <f>'OECD VAL'!X9*10^6*About!$A$25</f>
         <v>443551633131.10876</v>
       </c>
-      <c r="X2">
-        <f>'OECD VAL'!Y9*10^6*About!$A$14</f>
+      <c r="Y2">
+        <f>'OECD VAL'!Y9*10^6*About!$A$25</f>
         <v>1092867487465.397</v>
       </c>
-      <c r="Y2">
-        <f>'OECD VAL'!Z9*10^6*About!$A$14</f>
+      <c r="Z2">
+        <f>'OECD VAL'!Z9*10^6*About!$A$25</f>
         <v>358730084291.4812</v>
       </c>
-      <c r="Z2">
-        <f>'OECD VAL'!AA9*10^6*About!$A$14</f>
+      <c r="AA2">
+        <f>'OECD VAL'!AA9*10^6*About!$A$25</f>
         <v>330227698478.54797</v>
       </c>
-      <c r="AA2">
-        <f>'OECD VAL'!AB9*10^6*About!$A$14</f>
+      <c r="AB2">
+        <f>'OECD VAL'!AB9*10^6*About!$A$25</f>
         <v>197642858841.8468</v>
       </c>
-      <c r="AB2">
-        <f>'OECD VAL'!AC9*10^6*About!$A$14</f>
+      <c r="AC2">
+        <f>'OECD VAL'!AC9*10^6*About!$A$25</f>
         <v>83292175969.808075</v>
       </c>
-      <c r="AC2">
-        <f>'OECD VAL'!AD9*10^6*About!$A$14</f>
+      <c r="AD2">
+        <f>'OECD VAL'!AD9*10^6*About!$A$25</f>
         <v>286458782608.58081</v>
       </c>
-      <c r="AD2">
-        <f>'OECD VAL'!AE9*10^6*About!$A$14</f>
+      <c r="AE2">
+        <f>'OECD VAL'!AE9*10^6*About!$A$25</f>
         <v>726862913582.39282</v>
       </c>
-      <c r="AE2">
-        <f>'OECD VAL'!AF9*10^6*About!$A$14</f>
+      <c r="AF2">
+        <f>'OECD VAL'!AF9*10^6*About!$A$25</f>
         <v>99124994367.416687</v>
       </c>
-      <c r="AF2">
-        <f>'OECD VAL'!AG9*10^6*About!$A$14</f>
+      <c r="AG2">
+        <f>'OECD VAL'!AG9*10^6*About!$A$25</f>
         <v>1320219395505.2676</v>
       </c>
-      <c r="AG2">
-        <f>'OECD VAL'!AH9*10^6*About!$A$14</f>
+      <c r="AH2">
+        <f>'OECD VAL'!AH9*10^6*About!$A$25</f>
         <v>1182871631888.7844</v>
       </c>
-      <c r="AH2">
-        <f>'OECD VAL'!AI9*10^6*About!$A$14</f>
+      <c r="AI2">
+        <f>'OECD VAL'!AI9*10^6*About!$A$25</f>
         <v>838587376723.22241</v>
       </c>
-      <c r="AI2">
-        <f>'OECD VAL'!AJ9*10^6*About!$A$14</f>
+      <c r="AJ2">
+        <f>'OECD VAL'!AJ9*10^6*About!$A$25</f>
         <v>1041787952118.6583</v>
       </c>
-      <c r="AJ2">
-        <f>'OECD VAL'!AK9*10^6*About!$A$14</f>
+      <c r="AK2">
+        <f>'OECD VAL'!AK9*10^6*About!$A$25</f>
         <v>309954904850.23438</v>
       </c>
-      <c r="AK2">
-        <f>'OECD VAL'!AL9*10^6*About!$A$14</f>
+      <c r="AL2">
+        <f>'OECD VAL'!AL9*10^6*About!$A$25</f>
         <v>20682998307.294415</v>
       </c>
     </row>

</xml_diff>